<commit_message>
Added market research and analysis for task 2
</commit_message>
<xml_diff>
--- a/Spreadsheet_task2.xlsx
+++ b/Spreadsheet_task2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yusra Shahid\Documents\Bolt_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C3D100F-1786-4717-A6A6-25EEEC597E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA94B56-27B5-4B2E-8B0C-634796136C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{856AA51F-9F01-4945-A776-01D43DFD2972}"/>
   </bookViews>
@@ -147,8 +147,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -471,117 +471,116 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -899,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D639D2-5862-4292-BF77-CD750006A425}">
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -917,451 +916,410 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
     </row>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="44"/>
       <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="47"/>
     </row>
     <row r="5" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="3"/>
       <c r="D5" s="2"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="11"/>
+      <c r="F5" s="8"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-      <c r="F6" s="29" t="s">
+      <c r="C6" s="40"/>
+      <c r="D6" s="41"/>
+      <c r="F6" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="38"/>
     </row>
     <row r="7" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>9350000</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="7"/>
       <c r="F7" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="34">
         <f>80+7</f>
         <v>87</v>
       </c>
-      <c r="H7" s="11"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B8" s="8"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="9"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="11"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="7"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="5">
         <v>3500000</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" s="7"/>
       <c r="F9" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="35">
         <v>7</v>
       </c>
-      <c r="H9" s="11"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B10" s="8"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="9"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="11"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="7"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>300000</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="11"/>
+      <c r="D11" s="7"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>224000</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="F12" s="35" t="s">
+      <c r="D12" s="7"/>
+      <c r="F12" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12">
         <f>80*0.85</f>
         <v>68</v>
       </c>
-      <c r="H12" s="11"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="10">
         <v>184000</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="F13" s="10" t="s">
+      <c r="D13" s="7"/>
+      <c r="F13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13">
         <v>10</v>
       </c>
-      <c r="H13" s="11"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="5">
         <v>100000</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="F14" s="22" t="s">
+      <c r="D14" s="7"/>
+      <c r="F14" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="36">
+      <c r="G14" s="17">
         <f>G7-G9-G12-G13</f>
         <v>2</v>
       </c>
-      <c r="H14" s="23"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="10">
         <v>92000</v>
       </c>
-      <c r="D15" s="9"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B16" s="8"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="9"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="8" t="s">
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="6"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="5">
         <v>3200000</v>
       </c>
-      <c r="D17" s="9"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="8" t="s">
+      <c r="D17" s="7"/>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="5">
         <v>2400000</v>
       </c>
-      <c r="D18" s="9"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="8" t="s">
+      <c r="D18" s="7"/>
+      <c r="F18" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="10">
         <f>C18*92/100</f>
         <v>2208000</v>
       </c>
-      <c r="D19" s="9"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="8" t="s">
+      <c r="D19" s="7"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="5">
         <v>800000</v>
       </c>
-      <c r="D20" s="9"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="8" t="s">
+      <c r="D20" s="7"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="26"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="10">
         <f>C20*92.6/100</f>
         <v>740800</v>
       </c>
-      <c r="D21" s="9"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="8"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="19" t="s">
+      <c r="D21" s="7"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="6"/>
+      <c r="D22" s="7"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
+    </row>
+    <row r="23" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="12">
         <f>C13+C15+C19+C21</f>
         <v>3224800</v>
       </c>
-      <c r="D23" s="21"/>
-    </row>
-    <row r="24" spans="2:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D23" s="13"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="26"/>
+    </row>
+    <row r="24" spans="2:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="3"/>
       <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="2:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="12" t="s">
+      <c r="F24" s="24"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="26"/>
+    </row>
+    <row r="25" spans="2:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
-    </row>
-    <row r="26" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="8" t="s">
+      <c r="C25" s="40"/>
+      <c r="D25" s="41"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="26"/>
+    </row>
+    <row r="26" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="4">
         <v>3224800</v>
       </c>
-      <c r="D26" s="9"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="8" t="s">
+      <c r="D26" s="7"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="26"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B27" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="3">
         <v>0.44500000000000001</v>
       </c>
-      <c r="D27" s="9"/>
-    </row>
-    <row r="28" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="19" t="s">
+      <c r="D27" s="7"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="26"/>
+    </row>
+    <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="20">
+      <c r="C28" s="12">
         <f>C26*C27</f>
         <v>1435036</v>
       </c>
-      <c r="D28" s="21"/>
-    </row>
-    <row r="29" spans="2:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D28" s="13"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="26"/>
+    </row>
+    <row r="29" spans="2:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="1"/>
-      <c r="C29" s="3"/>
       <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="2:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="12" t="s">
+      <c r="F29" s="24"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="26"/>
+    </row>
+    <row r="30" spans="2:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-    </row>
-    <row r="31" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="8" t="s">
+      <c r="C30" s="40"/>
+      <c r="D30" s="41"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="26"/>
+    </row>
+    <row r="31" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="5">
         <v>1435036</v>
       </c>
-      <c r="D31" s="9"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B32" s="8" t="s">
+      <c r="D31" s="7"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="26"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B32" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32">
         <v>80</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="19" t="s">
+      <c r="F32" s="24"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="26"/>
+    </row>
+    <row r="33" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="20">
+      <c r="C33" s="12">
         <f>C32*C31</f>
         <v>114802880</v>
       </c>
-      <c r="D33" s="21"/>
-    </row>
-    <row r="34" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="38"/>
-      <c r="D37" s="39"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B38" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="41"/>
-      <c r="D38" s="42"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B39" s="43"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="45"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B40" s="43"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="45"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B41" s="43"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="45"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B42" s="43"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="45"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B43" s="43"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="45"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B44" s="43"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="45"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B45" s="43"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="45"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B46" s="43"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="45"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B47" s="43"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="45"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B48" s="43"/>
-      <c r="C48" s="44"/>
-      <c r="D48" s="45"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B49" s="43"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="45"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B50" s="43"/>
-      <c r="C50" s="44"/>
-      <c r="D50" s="45"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B51" s="43"/>
-      <c r="C51" s="44"/>
-      <c r="D51" s="45"/>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B52" s="43"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="45"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B53" s="43"/>
-      <c r="C53" s="44"/>
-      <c r="D53" s="45"/>
-    </row>
-    <row r="54" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="46"/>
-      <c r="C54" s="47"/>
-      <c r="D54" s="48"/>
-    </row>
-    <row r="55" spans="2:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="D33" s="13"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="26"/>
+    </row>
+    <row r="34" spans="2:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F34" s="27"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="29"/>
+    </row>
+    <row r="35" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D54"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H34"/>
     <mergeCell ref="B1:O2"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>

</xml_diff>